<commit_message>
acrescentado o sublinhado nas chaves primárias
</commit_message>
<xml_diff>
--- a/desafio02/desafio02.xlsx
+++ b/desafio02/desafio02.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c49175be73b77308/Área de Trabalho/Programação/BDD/desafio01/desafio02/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c49175be73b77308/Área de Trabalho/Programação/BDD/devsuperior/desafio02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB7A0E02-4246-45F5-83A2-728BF7B65336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{DB7A0E02-4246-45F5-83A2-728BF7B65336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2234B98-3BCA-4AD7-9014-128B6C285172}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B3374F3C-D189-4D48-8901-D8663AF26F49}"/>
   </bookViews>
@@ -79,18 +79,6 @@
     <t>funcionario_id referencia: tb_funcionario</t>
   </si>
   <si>
-    <t>(id, nome, email)</t>
-  </si>
-  <si>
-    <t>( valor_por_hora, horas, empreitada_id, funcionario_id)</t>
-  </si>
-  <si>
-    <t>(id, nome, telefone)</t>
-  </si>
-  <si>
-    <t>(id, nome)</t>
-  </si>
-  <si>
     <t>(funcionario_id, departamento_id)</t>
   </si>
   <si>
@@ -173,15 +161,140 @@
   <si>
     <t>Infraestrutura</t>
   </si>
+  <si>
+    <r>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, nome, telefone)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">( valor_por_hora, horas, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>empreitada_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>funcionario_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, nome, email)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, nome)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,12 +321,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF002060"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -259,6 +366,30 @@
       <b/>
       <sz val="11"/>
       <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -446,14 +577,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -463,40 +591,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -706,8 +840,8 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>94252</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>94768</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>180493</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -757,8 +891,8 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>218057</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>37744</xdr:rowOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>142519</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1100,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A35F0FDE-981F-4D33-901C-B742D108237D}">
   <dimension ref="B1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="U27" sqref="U27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,355 +1251,355 @@
   <sheetData>
     <row r="1" spans="2:21" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:21" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R2" s="14" t="s">
-        <v>20</v>
+      <c r="R2" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="S2" s="15"/>
-      <c r="T2" s="16"/>
-    </row>
-    <row r="3" spans="2:21" ht="15.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="T2" s="14"/>
+    </row>
+    <row r="3" spans="2:21" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R3" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="S3" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="T3" s="17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="2:21" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="R4" s="13">
+      <c r="R3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" s="10">
         <v>1</v>
       </c>
-      <c r="S4" s="13" t="s">
+      <c r="S4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="T4" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R5" s="10">
+        <v>2</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="T5" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="T4" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="2:21" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R5" s="13">
-        <v>2</v>
-      </c>
-      <c r="S5" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="T5" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="2:21" ht="15.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:21" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="R6" s="13">
+      <c r="R6" s="10">
         <v>3</v>
       </c>
-      <c r="S6" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="T6" s="13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="2:21" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="2:21" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="4" t="s">
+      <c r="S6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="T6" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="R8" s="14" t="s">
+      <c r="R8" s="13" t="s">
         <v>10</v>
       </c>
       <c r="S8" s="15"/>
       <c r="T8" s="15"/>
-      <c r="U8" s="16"/>
-    </row>
-    <row r="9" spans="2:21" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R9" s="17" t="s">
+      <c r="U8" s="14"/>
+    </row>
+    <row r="9" spans="2:21" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R9" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="S9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="T9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="S9" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="T9" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="U9" s="17" t="s">
+      <c r="U9" s="11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:21" ht="15.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="R10" s="10">
+      <c r="R10" s="7">
         <v>1</v>
       </c>
-      <c r="S10" s="11">
+      <c r="S10" s="8">
         <v>44640</v>
       </c>
-      <c r="T10" s="11">
+      <c r="T10" s="8">
         <v>44668</v>
       </c>
-      <c r="U10" s="10">
+      <c r="U10" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="R11" s="10">
+    <row r="11" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="R11" s="7">
         <v>2</v>
       </c>
-      <c r="S11" s="11">
+      <c r="S11" s="8">
         <v>44679</v>
       </c>
-      <c r="T11" s="11">
+      <c r="T11" s="8">
         <v>44696</v>
       </c>
-      <c r="U11" s="10">
+      <c r="U11" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
+    <row r="12" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="2:21" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="4" t="s">
+    <row r="13" spans="2:21" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:21" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R14" s="14" t="s">
+    <row r="14" spans="2:21" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R14" s="13" t="s">
         <v>5</v>
       </c>
       <c r="S14" s="15"/>
       <c r="T14" s="15"/>
-      <c r="U14" s="16"/>
-    </row>
-    <row r="15" spans="2:21" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R15" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="S15" s="17" t="s">
+      <c r="U14" s="14"/>
+    </row>
+    <row r="15" spans="2:21" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R15" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="S15" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="T15" s="17" t="s">
+      <c r="T15" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="U15" s="17" t="s">
+      <c r="U15" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="2:21" ht="15.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:21" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
       </c>
-      <c r="R16" s="12">
+      <c r="R16" s="9">
         <v>60</v>
       </c>
-      <c r="S16" s="10">
+      <c r="S16" s="7">
         <v>10</v>
       </c>
-      <c r="T16" s="10">
+      <c r="T16" s="7">
         <v>1</v>
       </c>
-      <c r="U16" s="10">
+      <c r="U16" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:21" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="R17" s="12">
+    <row r="17" spans="2:21" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R17" s="9">
         <v>50</v>
       </c>
-      <c r="S17" s="10">
+      <c r="S17" s="7">
         <v>20</v>
       </c>
-      <c r="T17" s="10">
+      <c r="T17" s="7">
         <v>1</v>
       </c>
-      <c r="U17" s="10">
+      <c r="U17" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:21" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R18" s="12">
+    <row r="18" spans="2:21" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R18" s="9">
         <v>60</v>
       </c>
-      <c r="S18" s="10">
+      <c r="S18" s="7">
         <v>15</v>
       </c>
-      <c r="T18" s="10">
+      <c r="T18" s="7">
         <v>2</v>
       </c>
-      <c r="U18" s="10">
+      <c r="U18" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:21" ht="15.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:21" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="R19" s="12">
+      <c r="R19" s="9">
         <v>70</v>
       </c>
-      <c r="S19" s="10">
+      <c r="S19" s="7">
         <v>20</v>
       </c>
-      <c r="T19" s="10">
+      <c r="T19" s="7">
         <v>2</v>
       </c>
-      <c r="U19" s="10">
+      <c r="U19" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:21" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="2:21" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R21" s="14" t="s">
-        <v>27</v>
+    <row r="20" spans="2:21" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R21" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="S21" s="15"/>
-      <c r="T21" s="16"/>
-    </row>
-    <row r="22" spans="2:21" ht="15.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="T21" s="14"/>
+    </row>
+    <row r="22" spans="2:21" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="R22" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="S22" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="T22" s="17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="2:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
+      <c r="R22" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="S22" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="R23" s="10">
+      <c r="T22" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="R23" s="7">
         <v>1</v>
       </c>
-      <c r="S23" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="T23" s="10">
+      <c r="S23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="T23" s="7">
         <v>222333444</v>
       </c>
     </row>
-    <row r="24" spans="2:21" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="3" t="s">
+    <row r="24" spans="2:21" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="2:21" ht="15.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="4" t="s">
+    <row r="25" spans="2:21" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R25" s="14" t="s">
+      <c r="R25" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="S25" s="16"/>
-    </row>
-    <row r="26" spans="2:21" ht="15.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="R26" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="S26" s="17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R27" s="13">
+      <c r="S25" s="14"/>
+    </row>
+    <row r="26" spans="2:21" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="R26" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="S26" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R27" s="10">
         <v>1</v>
       </c>
-      <c r="S27" s="13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R28" s="13">
+      <c r="S27" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R28" s="10">
         <v>2</v>
       </c>
-      <c r="S28" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
-    </row>
-    <row r="30" spans="2:21" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R30" s="14" t="s">
+      <c r="S28" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R29" s="16"/>
+      <c r="S29" s="16"/>
+      <c r="T29" s="16"/>
+    </row>
+    <row r="30" spans="2:21" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R30" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="S30" s="16"/>
-    </row>
-    <row r="31" spans="2:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="R31" s="17" t="s">
+      <c r="S30" s="14"/>
+    </row>
+    <row r="31" spans="2:21" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="R31" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="S31" s="17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R32" s="13">
+      <c r="S31" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R32" s="10">
         <v>1</v>
       </c>
-      <c r="S32" s="13">
+      <c r="S32" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="R33" s="13">
+    <row r="33" spans="18:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R33" s="10">
         <v>2</v>
       </c>
-      <c r="S33" s="13">
+      <c r="S33" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="18:19" ht="22.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R34" s="13">
+    <row r="34" spans="18:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R34" s="10">
         <v>3</v>
       </c>
-      <c r="S34" s="13">
+      <c r="S34" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="18:19" x14ac:dyDescent="0.25">
-      <c r="R35" s="13">
+    <row r="35" spans="18:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R35" s="10">
         <v>3</v>
       </c>
-      <c r="S35" s="13">
+      <c r="S35" s="10">
         <v>2</v>
       </c>
     </row>
@@ -1485,6 +1619,7 @@
     <hyperlink ref="T6" r:id="rId3" xr:uid="{8EE016D0-2353-4229-8A44-C09A235FBCB0}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>